<commit_message>
IE models now have separate nodes for each BC
</commit_message>
<xml_diff>
--- a/IE_models/Castledawson_Bridge_IEM_revB.xlsx
+++ b/IE_models/Castledawson_Bridge_IEM_revB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/Documents/WorkDocuments/Python/agnetwork/IE_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAA56F2-8C0D-C248-A58E-F13A86E97B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B20C9B2-183E-1A4E-8D21-F88009CAF02F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14320" windowHeight="7700" xr2:uid="{41EF06E5-D224-AC48-85A7-03741ACF90EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{41EF06E5-D224-AC48-85A7-03741ACF90EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="219">
   <si>
     <t>Element ID</t>
   </si>
@@ -714,7 +714,13 @@
     <t>BB, Z</t>
   </si>
   <si>
-    <t>DD, 1</t>
+    <t>DD, 2</t>
+  </si>
+  <si>
+    <t>DD, 3</t>
+  </si>
+  <si>
+    <t>Expansion joint</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EA39B3-DC91-914B-9042-786A21D22A90}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
@@ -2367,10 +2373,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2076CE62-05A5-B445-85CA-61E02B12840C}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2401,6 +2407,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2410,7 +2438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910BBFC3-9F34-C245-85CB-8F57706AA034}">
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
@@ -4167,7 +4195,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C61" s="2">
         <f>(TAN(-6)*D61)+X1</f>

</xml_diff>

<commit_message>
This is just a mess
</commit_message>
<xml_diff>
--- a/IE_models/Castledawson_Bridge_IEM_revB.xlsx
+++ b/IE_models/Castledawson_Bridge_IEM_revB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/Documents/WorkDocuments/Python/agnetwork/IE_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B20C9B2-183E-1A4E-8D21-F88009CAF02F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8416A9-A7AB-F04C-845F-C9A4722F5D74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{41EF06E5-D224-AC48-85A7-03741ACF90EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{41EF06E5-D224-AC48-85A7-03741ACF90EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="1" r:id="rId1"/>
@@ -727,7 +727,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1305,9 +1305,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EA39B3-DC91-914B-9042-786A21D22A90}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="6"/>
@@ -1322,7 +1322,7 @@
     <col min="11" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="51">
+    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="51">
+    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="51">
+    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="J4" s="15"/>
     </row>
-    <row r="5" spans="1:10" ht="51">
+    <row r="5" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="J5" s="15"/>
     </row>
-    <row r="6" spans="1:10" ht="51">
+    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="J6" s="15"/>
     </row>
-    <row r="7" spans="1:10" ht="51">
+    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="51">
+    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51">
+    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="51">
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>28</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="1:10" ht="51">
+    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="J11" s="15"/>
     </row>
-    <row r="12" spans="1:10" ht="51">
+    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
@@ -1694,7 +1694,7 @@
       </c>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="1:10" ht="51">
+    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="51">
+    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="51">
+    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="51">
+    <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
@@ -1820,7 +1820,7 @@
       </c>
       <c r="J16" s="15"/>
     </row>
-    <row r="17" spans="1:10" ht="51">
+    <row r="17" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="1:10" ht="51">
+    <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
@@ -1880,7 +1880,7 @@
       </c>
       <c r="J18" s="15"/>
     </row>
-    <row r="19" spans="1:10" ht="51">
+    <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="68">
+    <row r="20" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>72</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="51">
+    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>33</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="51">
+    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="51">
+    <row r="23" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="51">
+    <row r="24" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>33</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="85">
+    <row r="25" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>73</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="51">
+    <row r="26" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>34</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="51">
+    <row r="27" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>34</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="51">
+    <row r="28" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>34</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="51">
+    <row r="29" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>34</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="68">
+    <row r="30" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>74</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="85">
+    <row r="31" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>35</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="68">
+    <row r="32" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>101</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="68">
+    <row r="33" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>102</v>
       </c>
@@ -2375,17 +2375,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2076CE62-05A5-B445-85CA-61E02B12840C}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>218</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>218</v>
       </c>
@@ -2442,7 +2442,7 @@
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11" style="2"/>
     <col min="3" max="3" width="11.33203125" style="2" customWidth="1"/>
@@ -2454,7 +2454,7 @@
     <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="17" thickBot="1">
+    <row r="4" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="17" thickBot="1">
+    <row r="9" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="17" thickBot="1">
+    <row r="11" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="17" thickBot="1">
+    <row r="12" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>54.74</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4264,7 +4264,7 @@
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>